<commit_message>
Worked on american stout's water profile
</commit_message>
<xml_diff>
--- a/recipes/american stout/Ez water calculator 302 metric.xlsx
+++ b/recipes/american stout/Ez water calculator 302 metric.xlsx
@@ -1899,6 +1899,96 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1957,98 +2047,8 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="10"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="10"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4825,8 +4825,8 @@
   </sheetPr>
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4841,17 +4841,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="172" t="s">
+      <c r="C1" s="204" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="172"/>
-      <c r="J1" s="172"/>
-      <c r="K1" s="172"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="204"/>
+      <c r="K1" s="204"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4887,11 +4887,11 @@
       <c r="H3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="174" t="s">
+      <c r="I3" s="206" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="174"/>
-      <c r="K3" s="175">
+      <c r="J3" s="206"/>
+      <c r="K3" s="207">
         <v>1</v>
       </c>
       <c r="L3" s="1"/>
@@ -4916,11 +4916,11 @@
       <c r="H4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="173" t="s">
+      <c r="I4" s="205" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="173"/>
-      <c r="K4" s="175"/>
+      <c r="J4" s="205"/>
+      <c r="K4" s="207"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4978,11 +4978,11 @@
       <c r="F7" s="7"/>
       <c r="G7" s="10"/>
       <c r="H7" s="31"/>
-      <c r="I7" s="180" t="s">
+      <c r="I7" s="212" t="s">
         <v>110</v>
       </c>
-      <c r="J7" s="180"/>
-      <c r="K7" s="181"/>
+      <c r="J7" s="212"/>
+      <c r="K7" s="213"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4991,7 +4991,7 @@
         <v>143</v>
       </c>
       <c r="D8" s="13">
-        <v>12.8</v>
+        <v>14.4</v>
       </c>
       <c r="E8" s="13">
         <v>0</v>
@@ -4999,9 +4999,9 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="31"/>
-      <c r="I8" s="180"/>
-      <c r="J8" s="180"/>
-      <c r="K8" s="181"/>
+      <c r="I8" s="212"/>
+      <c r="J8" s="212"/>
+      <c r="K8" s="213"/>
     </row>
     <row r="9" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
@@ -5010,7 +5010,7 @@
       </c>
       <c r="D9" s="156">
         <f>D8/3.785412</f>
-        <v>3.3814020772375639</v>
+        <v>3.8040773368922589</v>
       </c>
       <c r="E9" s="156">
         <f>E8/3.785412</f>
@@ -5019,9 +5019,9 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="31"/>
-      <c r="I9" s="180"/>
-      <c r="J9" s="180"/>
-      <c r="K9" s="181"/>
+      <c r="I9" s="212"/>
+      <c r="J9" s="212"/>
+      <c r="K9" s="213"/>
     </row>
     <row r="10" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
@@ -5037,9 +5037,9 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="31"/>
-      <c r="I10" s="180"/>
-      <c r="J10" s="180"/>
-      <c r="K10" s="181"/>
+      <c r="I10" s="212"/>
+      <c r="J10" s="212"/>
+      <c r="K10" s="213"/>
     </row>
     <row r="11" spans="2:12" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="42"/>
@@ -5049,9 +5049,9 @@
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="45"/>
-      <c r="I11" s="182"/>
-      <c r="J11" s="182"/>
-      <c r="K11" s="183"/>
+      <c r="I11" s="214"/>
+      <c r="J11" s="214"/>
+      <c r="K11" s="215"/>
     </row>
     <row r="12" spans="2:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="59"/>
@@ -5125,7 +5125,7 @@
     </row>
     <row r="15" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="63"/>
-      <c r="C15" s="195" t="s">
+      <c r="C15" s="173" t="s">
         <v>118</v>
       </c>
       <c r="D15" s="66">
@@ -5154,7 +5154,7 @@
     </row>
     <row r="16" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="63"/>
-      <c r="C16" s="195"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="66">
         <v>11</v>
       </c>
@@ -5181,7 +5181,7 @@
     </row>
     <row r="17" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="63"/>
-      <c r="C17" s="195"/>
+      <c r="C17" s="173"/>
       <c r="D17" s="66">
         <v>11</v>
       </c>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="18" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="63"/>
-      <c r="C18" s="195"/>
+      <c r="C18" s="173"/>
       <c r="D18" s="66">
         <v>10</v>
       </c>
@@ -5235,7 +5235,7 @@
     </row>
     <row r="19" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="63"/>
-      <c r="C19" s="195"/>
+      <c r="C19" s="173"/>
       <c r="D19" s="66">
         <v>11</v>
       </c>
@@ -5262,7 +5262,7 @@
     </row>
     <row r="20" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="63"/>
-      <c r="C20" s="195"/>
+      <c r="C20" s="173"/>
       <c r="D20" s="66">
         <v>1</v>
       </c>
@@ -5289,7 +5289,7 @@
     </row>
     <row r="21" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="63"/>
-      <c r="C21" s="195"/>
+      <c r="C21" s="173"/>
       <c r="D21" s="66">
         <v>1</v>
       </c>
@@ -5316,7 +5316,7 @@
     </row>
     <row r="22" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="63"/>
-      <c r="C22" s="195"/>
+      <c r="C22" s="173"/>
       <c r="D22" s="66">
         <v>1</v>
       </c>
@@ -5343,7 +5343,7 @@
     </row>
     <row r="23" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="63"/>
-      <c r="C23" s="195"/>
+      <c r="C23" s="173"/>
       <c r="D23" s="66">
         <v>1</v>
       </c>
@@ -5380,12 +5380,12 @@
       </c>
       <c r="F24" s="69"/>
       <c r="G24" s="70"/>
-      <c r="H24" s="200" t="s">
+      <c r="H24" s="179" t="s">
         <v>133</v>
       </c>
-      <c r="I24" s="201"/>
-      <c r="J24" s="201"/>
-      <c r="K24" s="202"/>
+      <c r="I24" s="180"/>
+      <c r="J24" s="180"/>
+      <c r="K24" s="181"/>
     </row>
     <row r="25" spans="2:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="63"/>
@@ -5399,10 +5399,10 @@
       </c>
       <c r="F25" s="126"/>
       <c r="G25" s="70"/>
-      <c r="H25" s="201"/>
-      <c r="I25" s="201"/>
-      <c r="J25" s="201"/>
-      <c r="K25" s="202"/>
+      <c r="H25" s="180"/>
+      <c r="I25" s="180"/>
+      <c r="J25" s="180"/>
+      <c r="K25" s="181"/>
     </row>
     <row r="26" spans="2:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="63"/>
@@ -5412,14 +5412,14 @@
       </c>
       <c r="E26" s="152" t="str">
         <f>ROUND(D8/E24,2)&amp;" l/kg"</f>
-        <v>5,14 l/kg</v>
+        <v>5,78 l/kg</v>
       </c>
       <c r="F26" s="126"/>
       <c r="G26" s="70"/>
-      <c r="H26" s="201"/>
-      <c r="I26" s="201"/>
-      <c r="J26" s="201"/>
-      <c r="K26" s="202"/>
+      <c r="H26" s="180"/>
+      <c r="I26" s="180"/>
+      <c r="J26" s="180"/>
+      <c r="K26" s="181"/>
     </row>
     <row r="27" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="71"/>
@@ -5427,14 +5427,14 @@
       <c r="D27" s="151"/>
       <c r="E27" s="128" t="str">
         <f>ROUND(D9*4/E25,2)&amp;" qt/lb"</f>
-        <v>2,46 qt/lb</v>
+        <v>2,77 qt/lb</v>
       </c>
       <c r="F27" s="123"/>
       <c r="G27" s="123"/>
-      <c r="H27" s="203"/>
-      <c r="I27" s="203"/>
-      <c r="J27" s="203"/>
-      <c r="K27" s="204"/>
+      <c r="H27" s="182"/>
+      <c r="I27" s="182"/>
+      <c r="J27" s="182"/>
+      <c r="K27" s="183"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5446,55 +5446,55 @@
       <c r="E28" s="111"/>
       <c r="F28" s="112"/>
       <c r="G28" s="112"/>
-      <c r="H28" s="190" t="s">
+      <c r="H28" s="222" t="s">
         <v>139</v>
       </c>
-      <c r="I28" s="190"/>
-      <c r="J28" s="190"/>
-      <c r="K28" s="191"/>
+      <c r="I28" s="222"/>
+      <c r="J28" s="222"/>
+      <c r="K28" s="223"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="106"/>
       <c r="C29" s="108"/>
-      <c r="D29" s="178" t="s">
+      <c r="D29" s="210" t="s">
         <v>136</v>
       </c>
-      <c r="E29" s="218" t="s">
+      <c r="E29" s="197" t="s">
         <v>137</v>
       </c>
-      <c r="F29" s="186" t="s">
+      <c r="F29" s="218" t="s">
         <v>128</v>
       </c>
-      <c r="G29" s="188" t="s">
+      <c r="G29" s="220" t="s">
         <v>129</v>
       </c>
-      <c r="H29" s="192"/>
-      <c r="I29" s="192"/>
-      <c r="J29" s="192"/>
-      <c r="K29" s="193"/>
+      <c r="H29" s="174"/>
+      <c r="I29" s="174"/>
+      <c r="J29" s="174"/>
+      <c r="K29" s="224"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="106"/>
       <c r="C30" s="114"/>
-      <c r="D30" s="178"/>
-      <c r="E30" s="219"/>
-      <c r="F30" s="186"/>
-      <c r="G30" s="188"/>
-      <c r="H30" s="192"/>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
-      <c r="K30" s="193"/>
+      <c r="D30" s="210"/>
+      <c r="E30" s="198"/>
+      <c r="F30" s="218"/>
+      <c r="G30" s="220"/>
+      <c r="H30" s="174"/>
+      <c r="I30" s="174"/>
+      <c r="J30" s="174"/>
+      <c r="K30" s="224"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="106"/>
       <c r="C31" s="107"/>
-      <c r="D31" s="179"/>
-      <c r="E31" s="220"/>
-      <c r="F31" s="187"/>
-      <c r="G31" s="189"/>
+      <c r="D31" s="211"/>
+      <c r="E31" s="199"/>
+      <c r="F31" s="219"/>
+      <c r="G31" s="221"/>
       <c r="H31" s="120"/>
       <c r="I31" s="120"/>
       <c r="J31" s="120"/>
@@ -5506,25 +5506,25 @@
       <c r="C32" s="115"/>
       <c r="D32" s="116">
         <f>(1-D$10)*I$5*IF(K$3=1,50/61,IF(OR(K$3=0,K$3=2),1,"ERROR"))+(F$44*130+E$44*157-176.1*J37*J36*2-4160.4*H36*H38*2.5+D$44*357)/D$9</f>
-        <v>-113.91357117950818</v>
+        <v>-86.138110629508191</v>
       </c>
       <c r="E32" s="117">
         <f>D32-((D51/1.4)+(E51/1.7))</f>
-        <v>-203.07702959337371</v>
+        <v>-169.67182903286954</v>
       </c>
       <c r="F32" s="118">
         <f>(E15*G15+E16*G16+E17*G17+E18*G18+E19*G19+E20*G20+E21*G21+E22*G22+E23*G23)/E24+(0.1085*D9/E25+0.013)*E32/50</f>
-        <v>5.2360426195660086</v>
+        <v>5.2610302678274641</v>
       </c>
       <c r="G32" s="119" t="s">
         <v>93</v>
       </c>
-      <c r="H32" s="192" t="s">
+      <c r="H32" s="174" t="s">
         <v>132</v>
       </c>
-      <c r="I32" s="196"/>
-      <c r="J32" s="196"/>
-      <c r="K32" s="197"/>
+      <c r="I32" s="175"/>
+      <c r="J32" s="175"/>
+      <c r="K32" s="176"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="2:12" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5534,10 +5534,10 @@
       <c r="E33" s="130"/>
       <c r="F33" s="130"/>
       <c r="G33" s="138"/>
-      <c r="H33" s="198"/>
-      <c r="I33" s="198"/>
-      <c r="J33" s="198"/>
-      <c r="K33" s="199"/>
+      <c r="H33" s="177"/>
+      <c r="I33" s="177"/>
+      <c r="J33" s="177"/>
+      <c r="K33" s="178"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5713,13 +5713,13 @@
       <c r="D41" s="96"/>
       <c r="E41" s="96"/>
       <c r="F41" s="96"/>
-      <c r="G41" s="208" t="s">
+      <c r="G41" s="187" t="s">
         <v>130</v>
       </c>
-      <c r="H41" s="208"/>
-      <c r="I41" s="208"/>
-      <c r="J41" s="208"/>
-      <c r="K41" s="209"/>
+      <c r="H41" s="187"/>
+      <c r="I41" s="187"/>
+      <c r="J41" s="187"/>
+      <c r="K41" s="188"/>
     </row>
     <row r="42" spans="2:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="90"/>
@@ -5733,11 +5733,11 @@
       <c r="F42" s="97" t="s">
         <v>111</v>
       </c>
-      <c r="G42" s="210"/>
-      <c r="H42" s="210"/>
-      <c r="I42" s="210"/>
-      <c r="J42" s="210"/>
-      <c r="K42" s="211"/>
+      <c r="G42" s="189"/>
+      <c r="H42" s="189"/>
+      <c r="I42" s="189"/>
+      <c r="J42" s="189"/>
+      <c r="K42" s="190"/>
     </row>
     <row r="43" spans="2:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="80"/>
@@ -5753,11 +5753,11 @@
       <c r="F43" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="G43" s="210"/>
-      <c r="H43" s="210"/>
-      <c r="I43" s="210"/>
-      <c r="J43" s="210"/>
-      <c r="K43" s="211"/>
+      <c r="G43" s="189"/>
+      <c r="H43" s="189"/>
+      <c r="I43" s="189"/>
+      <c r="J43" s="189"/>
+      <c r="K43" s="190"/>
     </row>
     <row r="44" spans="2:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="90"/>
@@ -5870,10 +5870,10 @@
       <c r="H49" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I49" s="185" t="s">
+      <c r="I49" s="217" t="s">
         <v>138</v>
       </c>
-      <c r="J49" s="185"/>
+      <c r="J49" s="217"/>
       <c r="K49" s="49"/>
       <c r="L49" s="1"/>
     </row>
@@ -5895,10 +5895,10 @@
       <c r="H50" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I50" s="184" t="s">
+      <c r="I50" s="216" t="s">
         <v>57</v>
       </c>
-      <c r="J50" s="184"/>
+      <c r="J50" s="216"/>
       <c r="K50" s="52"/>
       <c r="L50" s="19"/>
       <c r="M50" s="2"/>
@@ -5910,11 +5910,11 @@
       </c>
       <c r="D51" s="53">
         <f>(1-D$10)*D$5+(F$44*105.89+D$37*60+E$37*72+D$44*143)/D$9</f>
-        <v>115.54347462499999</v>
+        <v>108.327533</v>
       </c>
       <c r="E51" s="53">
         <f>(1-D$10)*E$5+F$37*24.6/D$9</f>
-        <v>11.275088687499998</v>
+        <v>10.466745500000002</v>
       </c>
       <c r="F51" s="53">
         <f>(1-D$10)*F$5+E$44*72.3/D$9</f>
@@ -5922,17 +5922,17 @@
       </c>
       <c r="G51" s="53">
         <f>(1-D$10)*G$5+E$37*127.47/D$9</f>
-        <v>71.855284511874999</v>
+        <v>64.315808454999996</v>
       </c>
       <c r="H51" s="53">
         <f>(1-D$10)*H$5+(D$37*147.4+F$37*103)/D$9</f>
-        <v>102.34781478124999</v>
-      </c>
-      <c r="I51" s="216">
+        <v>91.698057583333338</v>
+      </c>
+      <c r="I51" s="195">
         <f>G51/H51</f>
-        <v>0.70206955239301116</v>
-      </c>
-      <c r="J51" s="217"/>
+        <v>0.70138681396332836</v>
+      </c>
+      <c r="J51" s="196"/>
       <c r="K51" s="11"/>
     </row>
     <row r="52" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5942,11 +5942,11 @@
       </c>
       <c r="D52" s="54">
         <f>IF(E8=0,D51,(1-(((D$10*D$9)+(E$10*E$9))/(D$9+E$9)))*D$5+((F$44+F$46)*105.89+(D$37+D$39)*60+(E$37+E$39)*72+(D$44+D$46)*143)/(D$9+E$9))</f>
-        <v>115.54347462499999</v>
+        <v>108.327533</v>
       </c>
       <c r="E52" s="54">
         <f>IF(E8=0,E51,(1-(((D$10*D$9)+(E$10*E$9))/(D$9+E$9)))*E$5+(F$37+F$39)*24.6/(D$9+E$9))</f>
-        <v>11.275088687499998</v>
+        <v>10.466745500000002</v>
       </c>
       <c r="F52" s="54">
         <f>IF(E8=0,F51,(1-(((D$10*D$9)+(E$10*E$9))/(D$9+E$9)))*F$5+(E$44+E$46)*72.3/(D$9+E$9))</f>
@@ -5954,17 +5954,17 @@
       </c>
       <c r="G52" s="54">
         <f>IF(E8=0,G51,(1-(((D$10*D$9)+(E$10*E$9))/(D$9+E$9)))*G$5+(E$37+E$39)*127.47/(D$9+E$9))</f>
-        <v>71.855284511874999</v>
+        <v>64.315808454999996</v>
       </c>
       <c r="H52" s="54">
         <f>IF(E8=0,H51,(1-(((D$10*D$9)+(E$10*E$9))/(D$9+E$9)))*H$5+((D$37+D$39)*147.4+(F$37+F$39)*103)/(D$9+E$9))</f>
-        <v>102.34781478124999</v>
-      </c>
-      <c r="I52" s="176">
+        <v>91.698057583333338</v>
+      </c>
+      <c r="I52" s="208">
         <f>G52/H52</f>
-        <v>0.70206955239301116</v>
-      </c>
-      <c r="J52" s="177"/>
+        <v>0.70138681396332836</v>
+      </c>
+      <c r="J52" s="209"/>
       <c r="K52" s="11"/>
       <c r="M52" s="1"/>
     </row>
@@ -5988,42 +5988,42 @@
       <c r="H53" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="I53" s="214" t="str">
+      <c r="I53" s="193" t="str">
         <f>IF(I52&lt;0.77,"Below .77, May enhance bitterness", IF(I52&lt;1.3,".77 to 1.3 = Balanced","Above 1.3 may enhance maltiness"))</f>
         <v>Below .77, May enhance bitterness</v>
       </c>
-      <c r="J53" s="215"/>
+      <c r="J53" s="194"/>
       <c r="K53" s="49"/>
       <c r="L53" s="1"/>
     </row>
     <row r="54" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="6"/>
-      <c r="C54" s="212" t="s">
+      <c r="C54" s="191" t="s">
         <v>131</v>
       </c>
-      <c r="D54" s="212"/>
-      <c r="E54" s="212"/>
-      <c r="F54" s="212"/>
-      <c r="G54" s="212"/>
-      <c r="H54" s="212"/>
-      <c r="I54" s="212"/>
-      <c r="J54" s="212"/>
-      <c r="K54" s="213"/>
+      <c r="D54" s="191"/>
+      <c r="E54" s="191"/>
+      <c r="F54" s="191"/>
+      <c r="G54" s="191"/>
+      <c r="H54" s="191"/>
+      <c r="I54" s="191"/>
+      <c r="J54" s="191"/>
+      <c r="K54" s="192"/>
       <c r="L54" s="1"/>
       <c r="M54" s="2"/>
       <c r="N54" s="19"/>
     </row>
     <row r="55" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
-      <c r="C55" s="205"/>
-      <c r="D55" s="205"/>
-      <c r="E55" s="205"/>
-      <c r="F55" s="205"/>
-      <c r="G55" s="205"/>
-      <c r="H55" s="205"/>
-      <c r="I55" s="206"/>
-      <c r="J55" s="206"/>
-      <c r="K55" s="207"/>
+      <c r="C55" s="184"/>
+      <c r="D55" s="184"/>
+      <c r="E55" s="184"/>
+      <c r="F55" s="184"/>
+      <c r="G55" s="184"/>
+      <c r="H55" s="184"/>
+      <c r="I55" s="185"/>
+      <c r="J55" s="185"/>
+      <c r="K55" s="186"/>
     </row>
     <row r="56" spans="1:14" s="167" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="168"/>
@@ -6039,17 +6039,17 @@
     </row>
     <row r="57" spans="1:14" s="167" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="168"/>
-      <c r="C57" s="224" t="s">
+      <c r="C57" s="203" t="s">
         <v>157</v>
       </c>
-      <c r="D57" s="224"/>
-      <c r="E57" s="224"/>
-      <c r="F57" s="224"/>
-      <c r="G57" s="224"/>
-      <c r="H57" s="224"/>
-      <c r="I57" s="224"/>
-      <c r="J57" s="224"/>
-      <c r="K57" s="224"/>
+      <c r="D57" s="203"/>
+      <c r="E57" s="203"/>
+      <c r="F57" s="203"/>
+      <c r="G57" s="203"/>
+      <c r="H57" s="203"/>
+      <c r="I57" s="203"/>
+      <c r="J57" s="203"/>
+      <c r="K57" s="203"/>
     </row>
     <row r="58" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="160"/>
@@ -6147,42 +6147,42 @@
       <c r="K64" s="163"/>
     </row>
     <row r="65" spans="1:11" s="166" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="223" t="s">
+      <c r="C65" s="202" t="s">
         <v>58</v>
       </c>
-      <c r="D65" s="223"/>
-      <c r="E65" s="223"/>
-      <c r="F65" s="223"/>
-      <c r="G65" s="223"/>
-      <c r="H65" s="223"/>
-      <c r="I65" s="223"/>
-      <c r="J65" s="223"/>
+      <c r="D65" s="202"/>
+      <c r="E65" s="202"/>
+      <c r="F65" s="202"/>
+      <c r="G65" s="202"/>
+      <c r="H65" s="202"/>
+      <c r="I65" s="202"/>
+      <c r="J65" s="202"/>
     </row>
     <row r="66" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="222" t="s">
+      <c r="C66" s="201" t="s">
         <v>134</v>
       </c>
-      <c r="D66" s="222"/>
-      <c r="E66" s="222"/>
-      <c r="F66" s="222"/>
-      <c r="G66" s="222"/>
-      <c r="H66" s="222"/>
-      <c r="I66" s="222"/>
-      <c r="J66" s="222"/>
-      <c r="K66" s="222"/>
+      <c r="D66" s="201"/>
+      <c r="E66" s="201"/>
+      <c r="F66" s="201"/>
+      <c r="G66" s="201"/>
+      <c r="H66" s="201"/>
+      <c r="I66" s="201"/>
+      <c r="J66" s="201"/>
+      <c r="K66" s="201"/>
     </row>
     <row r="67" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="221" t="s">
+      <c r="C67" s="200" t="s">
         <v>135</v>
       </c>
-      <c r="D67" s="221"/>
-      <c r="E67" s="221"/>
-      <c r="F67" s="221"/>
-      <c r="G67" s="221"/>
-      <c r="H67" s="221"/>
-      <c r="I67" s="221"/>
-      <c r="J67" s="221"/>
-      <c r="K67" s="221"/>
+      <c r="D67" s="200"/>
+      <c r="E67" s="200"/>
+      <c r="F67" s="200"/>
+      <c r="G67" s="200"/>
+      <c r="H67" s="200"/>
+      <c r="I67" s="200"/>
+      <c r="J67" s="200"/>
+      <c r="K67" s="200"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="38"/>
@@ -6200,16 +6200,16 @@
       <c r="K68" s="39"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C69" s="194" t="s">
+      <c r="C69" s="172" t="s">
         <v>125</v>
       </c>
-      <c r="D69" s="194"/>
-      <c r="E69" s="194"/>
-      <c r="F69" s="194"/>
-      <c r="G69" s="194"/>
-      <c r="H69" s="194"/>
-      <c r="I69" s="194"/>
-      <c r="J69" s="194"/>
+      <c r="D69" s="172"/>
+      <c r="E69" s="172"/>
+      <c r="F69" s="172"/>
+      <c r="G69" s="172"/>
+      <c r="H69" s="172"/>
+      <c r="I69" s="172"/>
+      <c r="J69" s="172"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C70" s="3" t="s">
@@ -6224,16 +6224,16 @@
       <c r="J70" s="58"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C71" s="194" t="s">
+      <c r="C71" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="D71" s="194"/>
-      <c r="E71" s="194"/>
-      <c r="F71" s="194"/>
-      <c r="G71" s="194"/>
-      <c r="H71" s="194"/>
-      <c r="I71" s="194"/>
-      <c r="J71" s="194"/>
+      <c r="D71" s="172"/>
+      <c r="E71" s="172"/>
+      <c r="F71" s="172"/>
+      <c r="G71" s="172"/>
+      <c r="H71" s="172"/>
+      <c r="I71" s="172"/>
+      <c r="J71" s="172"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C73" s="28" t="s">
@@ -6252,6 +6252,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="I7:K11"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="H28:K30"/>
     <mergeCell ref="C69:J69"/>
     <mergeCell ref="C71:J71"/>
     <mergeCell ref="C15:C23"/>
@@ -6267,18 +6279,6 @@
     <mergeCell ref="C66:K66"/>
     <mergeCell ref="C65:J65"/>
     <mergeCell ref="C57:K57"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="I7:K11"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="H28:K30"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D53">
@@ -6743,7 +6743,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6824,7 +6824,7 @@
       </c>
       <c r="B11" s="1">
         <f>'EZ Water Adjustment'!D8</f>
-        <v>12.8</v>
+        <v>14.4</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>48</v>
@@ -6978,14 +6978,14 @@
       </c>
       <c r="B26" s="26">
         <f>'EZ Water Adjustment'!D51</f>
-        <v>115.54347462499999</v>
+        <v>108.327533</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="26">
         <f>'EZ Water Adjustment'!D52</f>
-        <v>115.54347462499999</v>
+        <v>108.327533</v>
       </c>
       <c r="I26" s="26"/>
     </row>
@@ -6995,14 +6995,14 @@
       </c>
       <c r="B27" s="26">
         <f>'EZ Water Adjustment'!E51</f>
-        <v>11.275088687499998</v>
+        <v>10.466745500000002</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="26">
         <f>'EZ Water Adjustment'!E52</f>
-        <v>11.275088687499998</v>
+        <v>10.466745500000002</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -7027,14 +7027,14 @@
       </c>
       <c r="B29" s="26">
         <f>'EZ Water Adjustment'!G51</f>
-        <v>71.855284511874999</v>
+        <v>64.315808454999996</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D29" s="26">
         <f>'EZ Water Adjustment'!G52</f>
-        <v>71.855284511874999</v>
+        <v>64.315808454999996</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -7043,14 +7043,14 @@
       </c>
       <c r="B30" s="26">
         <f>'EZ Water Adjustment'!H51</f>
-        <v>102.34781478124999</v>
+        <v>91.698057583333338</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D30" s="26">
         <f>'EZ Water Adjustment'!H52</f>
-        <v>102.34781478124999</v>
+        <v>91.698057583333338</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -7059,14 +7059,14 @@
       </c>
       <c r="B31" s="27">
         <f>'EZ Water Adjustment'!I51</f>
-        <v>0.70206955239301116</v>
+        <v>0.70138681396332836</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D31" s="27">
         <f>'EZ Water Adjustment'!I52</f>
-        <v>0.70206955239301116</v>
+        <v>0.70138681396332836</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -7079,7 +7079,7 @@
       </c>
       <c r="B33" s="26">
         <f>'EZ Water Adjustment'!D32</f>
-        <v>-113.91357117950818</v>
+        <v>-86.138110629508191</v>
       </c>
       <c r="C33" s="3"/>
     </row>
@@ -7089,7 +7089,7 @@
       </c>
       <c r="B34" s="26">
         <f>'EZ Water Adjustment'!E32</f>
-        <v>-203.07702959337371</v>
+        <v>-169.67182903286954</v>
       </c>
       <c r="C34" s="3"/>
     </row>
@@ -7099,7 +7099,7 @@
       </c>
       <c r="B35" s="27">
         <f>'EZ Water Adjustment'!F32</f>
-        <v>5.2360426195660086</v>
+        <v>5.2610302678274641</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>